<commit_message>
wsr summary and links for navigation in all pages
</commit_message>
<xml_diff>
--- a/dataSources/WSR/CORPORATE_ACTIONS.xlsx
+++ b/dataSources/WSR/CORPORATE_ACTIONS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VigneshD\repository\vsCode\qaDash\dataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VigneshD\repository\vsCode\KMDV-Dash\dataSources\WSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="600" documentId="13_ncr:1_{0F8C332E-20C7-4FE6-8FBC-D589C740ED26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B159E512-1732-4624-8062-F4AC1B0F5CEF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DD5B14-52ED-449A-9566-126BA7D43BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="140">
   <si>
     <t>Task Name</t>
   </si>
@@ -536,7 +536,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1336,43 +1336,43 @@
   </sheetPr>
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="73.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="4"/>
-    <col min="12" max="12" width="89.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="4"/>
-    <col min="18" max="18" width="65.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="8.85546875" style="4"/>
-    <col min="28" max="28" width="16.5703125" style="4" customWidth="1"/>
-    <col min="29" max="29" width="15.7109375" style="4" customWidth="1"/>
-    <col min="30" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="17.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="4"/>
+    <col min="4" max="4" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="4"/>
+    <col min="7" max="7" width="73.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="4"/>
+    <col min="12" max="12" width="89.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="4"/>
+    <col min="18" max="18" width="65.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="8.88671875" style="4"/>
+    <col min="28" max="28" width="16.5546875" style="4" customWidth="1"/>
+    <col min="29" max="29" width="15.6640625" style="4" customWidth="1"/>
+    <col min="30" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="45.75">
+    <row r="2" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>23</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>33</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>39</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A5" s="29" t="s">
         <v>45</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>51</v>
       </c>
@@ -1664,19 +1664,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z7" s="23" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
         <v>55</v>
@@ -1685,45 +1681,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="30.75">
+    <row r="8" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>56</v>
       </c>
       <c r="B8" s="5">
         <v>8</v>
       </c>
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC8" s="27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29">
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1735,40 +1715,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436EB9FA-52AE-4AD4-9F71-F53D4D7CFCF9}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+    <sheetView topLeftCell="R5" workbookViewId="0">
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="8"/>
-    <col min="4" max="4" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
-    <col min="7" max="7" width="73.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="8"/>
-    <col min="12" max="12" width="89.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="8"/>
-    <col min="18" max="18" width="65.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="17.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="8"/>
+    <col min="4" max="4" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="8"/>
+    <col min="7" max="7" width="73.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="8"/>
+    <col min="12" max="12" width="89.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="8"/>
+    <col min="18" max="18" width="65.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="12" customFormat="1">
+    <row r="1" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1840,7 +1820,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="33">
+    <row r="2" spans="1:29" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A2" s="48" t="s">
         <v>113</v>
       </c>
@@ -1905,7 +1885,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>114</v>
       </c>
@@ -1960,7 +1940,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A4" s="25" t="s">
         <v>116</v>
       </c>
@@ -2007,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>117</v>
       </c>
@@ -2058,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>51</v>
       </c>
@@ -2109,7 +2089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>119</v>
       </c>
@@ -2146,9 +2126,7 @@
       <c r="V7" s="68"/>
       <c r="W7" s="68"/>
       <c r="X7" s="68"/>
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y7" s="25"/>
       <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
@@ -2158,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="30.75">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="68"/>
       <c r="B8" s="67"/>
       <c r="C8" s="68"/>
@@ -2191,21 +2169,15 @@
       <c r="V8" s="68"/>
       <c r="W8" s="68"/>
       <c r="X8" s="68"/>
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB8" s="27"/>
       <c r="AC8" s="27"/>
     </row>
-    <row r="9" spans="1:29" ht="30.75">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="68"/>
       <c r="B9" s="67"/>
       <c r="C9" s="68"/>
@@ -2238,21 +2210,15 @@
       <c r="V9" s="68"/>
       <c r="W9" s="68"/>
       <c r="X9" s="68"/>
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
       <c r="AC9" s="27"/>
     </row>
-    <row r="10" spans="1:29" ht="30.75">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="68"/>
       <c r="B10" s="67"/>
       <c r="C10" s="68"/>
@@ -2291,7 +2257,7 @@
       <c r="AB10" s="68"/>
       <c r="AC10" s="68"/>
     </row>
-    <row r="11" spans="1:29" ht="30.75">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="68"/>
       <c r="B11" s="67"/>
       <c r="C11" s="68"/>
@@ -2330,7 +2296,7 @@
       <c r="AB11" s="68"/>
       <c r="AC11" s="68"/>
     </row>
-    <row r="12" spans="1:29" ht="30.75">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="68"/>
       <c r="B12" s="67"/>
       <c r="C12" s="68"/>
@@ -2369,7 +2335,7 @@
       <c r="AB12" s="68"/>
       <c r="AC12" s="68"/>
     </row>
-    <row r="13" spans="1:29" ht="30.75">
+    <row r="13" spans="1:29" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A13" s="68"/>
       <c r="B13" s="67"/>
       <c r="C13" s="68"/>
@@ -2406,7 +2372,7 @@
       <c r="AB13" s="68"/>
       <c r="AC13" s="68"/>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="68"/>
       <c r="B14" s="67"/>
       <c r="C14" s="68"/>
@@ -2446,40 +2412,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B89BFD8-A42D-4DA9-8F9C-388471437985}">
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+    <sheetView topLeftCell="U4" workbookViewId="0">
+      <selection activeCell="AB8" sqref="AB8:AC13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="8"/>
-    <col min="4" max="4" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
-    <col min="7" max="7" width="73.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="8"/>
-    <col min="12" max="12" width="89.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="8"/>
-    <col min="18" max="18" width="65.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="17.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="8"/>
+    <col min="4" max="4" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="8"/>
+    <col min="7" max="7" width="73.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="8"/>
+    <col min="12" max="12" width="89.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="8"/>
+    <col min="18" max="18" width="65.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="12" customFormat="1">
+    <row r="1" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2551,7 +2517,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="45.75">
+    <row r="2" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="46" t="s">
         <v>124</v>
       </c>
@@ -2608,7 +2574,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A3" s="50" t="s">
         <v>125</v>
       </c>
@@ -2659,7 +2625,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A4" s="50" t="s">
         <v>127</v>
       </c>
@@ -2710,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="67"/>
       <c r="C5" s="68"/>
@@ -2749,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="68"/>
       <c r="B6" s="67"/>
       <c r="C6" s="68"/>
@@ -2788,7 +2754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="68"/>
       <c r="B7" s="67"/>
       <c r="C7" s="68"/>
@@ -2813,12 +2779,8 @@
       <c r="V7" s="68"/>
       <c r="W7" s="68"/>
       <c r="X7" s="68"/>
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z7" s="23" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
         <v>55</v>
@@ -2827,7 +2789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="68"/>
       <c r="B8" s="67"/>
       <c r="C8" s="68"/>
@@ -2852,23 +2814,15 @@
       <c r="V8" s="68"/>
       <c r="W8" s="68"/>
       <c r="X8" s="68"/>
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC8" s="27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29">
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="68"/>
       <c r="B9" s="67"/>
       <c r="C9" s="68"/>
@@ -2893,21 +2847,13 @@
       <c r="V9" s="68"/>
       <c r="W9" s="68"/>
       <c r="X9" s="68"/>
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2918,40 +2864,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CD0AF5-EFB4-4E14-8A69-7FBCEBDF9AA4}">
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView topLeftCell="S5" workbookViewId="0">
+      <selection activeCell="AF10" sqref="AF10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="8"/>
-    <col min="4" max="4" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
-    <col min="7" max="7" width="73.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="8"/>
-    <col min="12" max="12" width="89.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="8"/>
-    <col min="18" max="18" width="65.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="17.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="8"/>
+    <col min="4" max="4" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="8"/>
+    <col min="7" max="7" width="73.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="8"/>
+    <col min="12" max="12" width="89.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="8"/>
+    <col min="18" max="18" width="65.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="12" customFormat="1">
+    <row r="1" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3023,7 +2969,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="45.75">
+    <row r="2" spans="1:29" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A2" s="46" t="s">
         <v>128</v>
       </c>
@@ -3084,7 +3030,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A3" s="50" t="s">
         <v>130</v>
       </c>
@@ -3131,7 +3077,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="50" t="s">
         <v>131</v>
       </c>
@@ -3174,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="67"/>
       <c r="C5" s="68"/>
@@ -3213,7 +3159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="68"/>
       <c r="B6" s="67"/>
       <c r="C6" s="68"/>
@@ -3252,7 +3198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="68"/>
       <c r="B7" s="67"/>
       <c r="C7" s="68"/>
@@ -3277,12 +3223,8 @@
       <c r="V7" s="68"/>
       <c r="W7" s="68"/>
       <c r="X7" s="68"/>
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z7" s="23" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
         <v>55</v>
@@ -3291,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="68"/>
       <c r="B8" s="67"/>
       <c r="C8" s="68"/>
@@ -3316,23 +3258,15 @@
       <c r="V8" s="68"/>
       <c r="W8" s="68"/>
       <c r="X8" s="68"/>
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC8" s="27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29">
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="68"/>
       <c r="B9" s="67"/>
       <c r="C9" s="68"/>
@@ -3357,21 +3291,13 @@
       <c r="V9" s="68"/>
       <c r="W9" s="68"/>
       <c r="X9" s="68"/>
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3382,40 +3308,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6FAE2C-B0F5-47D8-854F-03F354215233}">
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="8"/>
-    <col min="4" max="4" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
-    <col min="7" max="7" width="73.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="8"/>
-    <col min="12" max="12" width="89.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="8"/>
-    <col min="18" max="18" width="65.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="17.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="8"/>
+    <col min="4" max="4" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="8"/>
+    <col min="7" max="7" width="73.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="8"/>
+    <col min="12" max="12" width="89.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="8"/>
+    <col min="18" max="18" width="65.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="12" customFormat="1">
+    <row r="1" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3487,7 +3413,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="33">
+    <row r="2" spans="1:29" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A2" s="46" t="s">
         <v>132</v>
       </c>
@@ -3548,7 +3474,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A3" s="50"/>
       <c r="B3" s="49"/>
       <c r="C3" s="68"/>
@@ -3591,7 +3517,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="50"/>
       <c r="B4" s="49"/>
       <c r="C4" s="68"/>
@@ -3630,7 +3556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="67"/>
       <c r="C5" s="68"/>
@@ -3669,7 +3595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="68"/>
       <c r="B6" s="67"/>
       <c r="C6" s="68"/>
@@ -3708,7 +3634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="68"/>
       <c r="B7" s="67"/>
       <c r="C7" s="68"/>
@@ -3733,12 +3659,8 @@
       <c r="V7" s="68"/>
       <c r="W7" s="68"/>
       <c r="X7" s="68"/>
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z7" s="23" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
         <v>55</v>
@@ -3747,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="68"/>
       <c r="B8" s="67"/>
       <c r="C8" s="68"/>
@@ -3772,23 +3694,15 @@
       <c r="V8" s="68"/>
       <c r="W8" s="68"/>
       <c r="X8" s="68"/>
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC8" s="27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29">
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="68"/>
       <c r="B9" s="67"/>
       <c r="C9" s="68"/>
@@ -3813,21 +3727,13 @@
       <c r="V9" s="68"/>
       <c r="W9" s="68"/>
       <c r="X9" s="68"/>
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3838,40 +3744,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6724893F-E8A3-4F47-9556-9D519FBD597B}">
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="8"/>
-    <col min="4" max="4" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
-    <col min="7" max="7" width="73.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="8"/>
-    <col min="12" max="12" width="89.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="8"/>
-    <col min="18" max="18" width="65.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="17.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="8"/>
+    <col min="4" max="4" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="8"/>
+    <col min="7" max="7" width="73.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="8"/>
+    <col min="12" max="12" width="89.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="8"/>
+    <col min="18" max="18" width="65.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="12" customFormat="1">
+    <row r="1" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
@@ -3958,7 +3864,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="45.75">
+    <row r="2" spans="1:29" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A2" s="22" t="s">
         <v>133</v>
       </c>
@@ -4045,7 +3951,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>135</v>
       </c>
@@ -4055,12 +3961,8 @@
       <c r="C3" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>27</v>
-      </c>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="58" t="s">
         <v>27</v>
       </c>
@@ -4132,22 +4034,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
-      <c r="A4" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>27</v>
-      </c>
+    <row r="4" spans="1:29" ht="44.4" x14ac:dyDescent="0.4">
+      <c r="A4" s="50"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>27</v>
-      </c>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
       <c r="F4" s="58" t="s">
         <v>27</v>
       </c>
@@ -4211,22 +4105,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
-      <c r="A5" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="58" t="s">
-        <v>27</v>
-      </c>
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="64"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="58" t="s">
-        <v>27</v>
-      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
       <c r="F5" s="58" t="s">
         <v>27</v>
       </c>
@@ -4298,13 +4184,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
-      <c r="A6" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>27</v>
-      </c>
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="60"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="58" t="s">
         <v>27</v>
       </c>
@@ -4385,13 +4267,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
-      <c r="A7" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="58" t="s">
-        <v>27</v>
-      </c>
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="60"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="58" t="s">
         <v>27</v>
       </c>
@@ -4404,12 +4282,8 @@
       <c r="F7" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="66" t="s">
-        <v>27</v>
-      </c>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
       <c r="I7" s="66" t="s">
         <v>27</v>
       </c>
@@ -4458,12 +4332,8 @@
       <c r="X7" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="Y7" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z7" s="23" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
         <v>55</v>
@@ -4472,13 +4342,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
-      <c r="A8" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="58" t="s">
-        <v>27</v>
-      </c>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A8" s="60"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="58" t="s">
         <v>27</v>
       </c>
@@ -4491,12 +4357,8 @@
       <c r="F8" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="58" t="s">
-        <v>27</v>
-      </c>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
       <c r="I8" s="58" t="s">
         <v>27</v>
       </c>
@@ -4545,29 +4407,17 @@
       <c r="X8" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="Y8" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC8" s="27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29">
-      <c r="A9" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="58" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A9" s="60"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="58" t="s">
         <v>27</v>
       </c>
@@ -4580,12 +4430,8 @@
       <c r="F9" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="58" t="s">
-        <v>27</v>
-      </c>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
       <c r="I9" s="58" t="s">
         <v>27</v>
       </c>
@@ -4634,21 +4480,13 @@
       <c r="X9" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="Y9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4659,42 +4497,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D327FA-72B4-4A76-B935-E5D6BDEA8522}">
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+    <sheetView topLeftCell="R5" workbookViewId="0">
+      <selection activeCell="AB8" sqref="AB8:AC17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="8"/>
-    <col min="4" max="4" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
-    <col min="7" max="7" width="73.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="8"/>
-    <col min="12" max="12" width="89.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="8"/>
-    <col min="18" max="18" width="65.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="8.85546875" style="8"/>
-    <col min="29" max="29" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="17.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="8"/>
+    <col min="4" max="4" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="8"/>
+    <col min="7" max="7" width="73.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="8"/>
+    <col min="12" max="12" width="89.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="8"/>
+    <col min="18" max="18" width="65.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="8.88671875" style="8"/>
+    <col min="29" max="29" width="11.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="12" customFormat="1">
+    <row r="1" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4766,7 +4604,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="33">
+    <row r="2" spans="1:29" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A2" s="55" t="s">
         <v>138</v>
       </c>
@@ -4831,7 +4669,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A3" s="25"/>
       <c r="B3" s="49"/>
       <c r="C3" s="68"/>
@@ -4880,7 +4718,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A4" s="50"/>
       <c r="B4" s="49"/>
       <c r="C4" s="68"/>
@@ -4925,7 +4763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="67"/>
       <c r="C5" s="68"/>
@@ -4934,9 +4772,7 @@
       <c r="F5" s="68"/>
       <c r="G5" s="31"/>
       <c r="H5" s="33"/>
-      <c r="I5" s="33" t="s">
-        <v>27</v>
-      </c>
+      <c r="I5" s="33"/>
       <c r="J5" s="33" t="s">
         <v>27</v>
       </c>
@@ -4968,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="68"/>
       <c r="B6" s="67"/>
       <c r="C6" s="68"/>
@@ -5011,7 +4847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="68"/>
       <c r="B7" s="67"/>
       <c r="C7" s="68"/>
@@ -5036,9 +4872,7 @@
       <c r="V7" s="68"/>
       <c r="W7" s="68"/>
       <c r="X7" s="68"/>
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y7" s="25"/>
       <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
@@ -5048,7 +4882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="68"/>
       <c r="B8" s="67"/>
       <c r="C8" s="68"/>
@@ -5073,23 +4907,15 @@
       <c r="V8" s="68"/>
       <c r="W8" s="68"/>
       <c r="X8" s="68"/>
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC8" s="27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29">
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="68"/>
       <c r="B9" s="67"/>
       <c r="C9" s="68"/>
@@ -5114,21 +4940,13 @@
       <c r="V9" s="68"/>
       <c r="W9" s="68"/>
       <c r="X9" s="68"/>
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5142,40 +4960,40 @@
   </sheetPr>
   <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView topLeftCell="R5" workbookViewId="0">
+      <selection activeCell="AB8" sqref="AB8:AC11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="73.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="4"/>
-    <col min="12" max="12" width="89.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="4"/>
-    <col min="18" max="18" width="65.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="17.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="4"/>
+    <col min="4" max="4" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="4"/>
+    <col min="7" max="7" width="73.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="4"/>
+    <col min="12" max="12" width="89.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="4"/>
+    <col min="18" max="18" width="65.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5247,7 +5065,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="45.75">
+    <row r="2" spans="1:29" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A2" s="42" t="s">
         <v>57</v>
       </c>
@@ -5297,7 +5115,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
         <v>59</v>
       </c>
@@ -5348,7 +5166,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>60</v>
       </c>
@@ -5393,7 +5211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
         <v>51</v>
       </c>
@@ -5414,7 +5232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="45.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
         <v>62</v>
       </c>
@@ -5435,19 +5253,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="43" t="s">
         <v>63</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z7" s="23" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
         <v>55</v>
@@ -5456,51 +5270,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="30.75">
+    <row r="8" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="44" t="s">
         <v>64</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB8" s="27"/>
       <c r="AC8" s="27"/>
     </row>
-    <row r="9" spans="1:29" ht="45.75">
+    <row r="9" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="45" t="s">
         <v>65</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC9" s="27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" ht="30.75">
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
+    </row>
+    <row r="10" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="42" t="s">
         <v>66</v>
       </c>
@@ -5508,7 +5308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="45.75">
+    <row r="11" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="42" t="s">
         <v>67</v>
       </c>
@@ -5529,40 +5329,40 @@
   </sheetPr>
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView topLeftCell="S5" workbookViewId="0">
+      <selection activeCell="AG10" sqref="AG10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="73.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="4"/>
-    <col min="12" max="12" width="89.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="4"/>
-    <col min="18" max="18" width="65.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="17.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="4"/>
+    <col min="4" max="4" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="4"/>
+    <col min="7" max="7" width="73.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="4"/>
+    <col min="12" max="12" width="89.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="4"/>
+    <col min="18" max="18" width="65.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5634,7 +5434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="45.75">
+    <row r="2" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>68</v>
       </c>
@@ -5688,7 +5488,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>69</v>
       </c>
@@ -5739,7 +5539,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>71</v>
       </c>
@@ -5784,7 +5584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="73.2" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
       <c r="G5" s="39" t="s">
         <v>74</v>
@@ -5808,7 +5608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="G6"/>
       <c r="H6"/>
@@ -5828,13 +5628,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z7" s="23" t="s">
-        <v>27</v>
-      </c>
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
         <v>55</v>
@@ -5843,39 +5639,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC8" s="27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29">
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -5887,40 +5667,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B084B1D6-8D90-452D-8E2F-C931E1C70883}">
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView topLeftCell="R5" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="73.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="4"/>
-    <col min="12" max="12" width="89.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="4"/>
-    <col min="18" max="18" width="65.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="17.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="4"/>
+    <col min="4" max="4" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="4"/>
+    <col min="7" max="7" width="73.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="4"/>
+    <col min="12" max="12" width="89.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="4"/>
+    <col min="18" max="18" width="65.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5992,7 +5772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="30.75">
+    <row r="2" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>75</v>
       </c>
@@ -6036,7 +5816,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>76</v>
       </c>
@@ -6076,7 +5856,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>77</v>
       </c>
@@ -6109,7 +5889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>79</v>
       </c>
@@ -6130,7 +5910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>51</v>
       </c>
@@ -6151,13 +5931,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z7" s="23" t="s">
-        <v>27</v>
-      </c>
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
         <v>55</v>
@@ -6166,39 +5942,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC8" s="27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29">
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
+      <c r="AC9" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -6213,40 +5973,40 @@
   </sheetPr>
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView topLeftCell="R5" workbookViewId="0">
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="4"/>
-    <col min="4" max="4" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="4"/>
-    <col min="7" max="7" width="73.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="4"/>
-    <col min="12" max="12" width="89.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" style="4"/>
-    <col min="18" max="18" width="65.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="17.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="4"/>
+    <col min="4" max="4" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
+    <col min="7" max="7" width="73.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="4"/>
+    <col min="12" max="12" width="89.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="4"/>
+    <col min="18" max="18" width="65.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -6318,7 +6078,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="30.75">
+    <row r="2" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>75</v>
       </c>
@@ -6362,7 +6122,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>76</v>
       </c>
@@ -6402,7 +6162,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>77</v>
       </c>
@@ -6435,7 +6195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>79</v>
       </c>
@@ -6456,7 +6216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>51</v>
       </c>
@@ -6477,10 +6237,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Y7" s="25"/>
       <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
@@ -6490,34 +6248,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB8" s="27"/>
       <c r="AC8" s="27"/>
     </row>
-    <row r="9" spans="1:29">
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
       <c r="AC9" s="27"/>
     </row>
   </sheetData>
@@ -6533,40 +6279,40 @@
   </sheetPr>
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView topLeftCell="R5" workbookViewId="0">
+      <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="8"/>
-    <col min="4" max="4" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="8"/>
-    <col min="7" max="7" width="73.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="8"/>
-    <col min="12" max="12" width="89.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" style="8"/>
-    <col min="18" max="18" width="65.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="17.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="8"/>
+    <col min="4" max="4" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="8"/>
+    <col min="7" max="7" width="73.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="8"/>
+    <col min="12" max="12" width="89.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="8"/>
+    <col min="18" max="18" width="65.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="12" customFormat="1">
+    <row r="1" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -6638,7 +6384,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="45.75">
+    <row r="2" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
@@ -6695,7 +6441,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -6746,7 +6492,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="68"/>
       <c r="B4" s="67"/>
       <c r="C4" s="68"/>
@@ -6789,7 +6535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="68"/>
       <c r="B5" s="67"/>
       <c r="C5" s="68"/>
@@ -6828,7 +6574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="68"/>
       <c r="B6" s="67"/>
       <c r="C6" s="68"/>
@@ -6867,7 +6613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="68"/>
       <c r="B7" s="67"/>
       <c r="C7" s="68"/>
@@ -6892,9 +6638,7 @@
       <c r="V7" s="68"/>
       <c r="W7" s="68"/>
       <c r="X7" s="68"/>
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y7" s="25"/>
       <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
@@ -6904,7 +6648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="68"/>
       <c r="B8" s="67"/>
       <c r="C8" s="68"/>
@@ -6929,21 +6673,15 @@
       <c r="V8" s="68"/>
       <c r="W8" s="68"/>
       <c r="X8" s="68"/>
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB8" s="27"/>
       <c r="AC8" s="27"/>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="68"/>
       <c r="B9" s="67"/>
       <c r="C9" s="68"/>
@@ -6968,18 +6706,12 @@
       <c r="V9" s="68"/>
       <c r="W9" s="68"/>
       <c r="X9" s="68"/>
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
       <c r="AC9" s="27"/>
     </row>
   </sheetData>
@@ -6994,39 +6726,39 @@
   </sheetPr>
   <dimension ref="A1:AC18"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AG4" sqref="AG4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="4"/>
-    <col min="4" max="4" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="4"/>
-    <col min="7" max="7" width="73.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="4"/>
-    <col min="12" max="12" width="89.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.85546875" style="4"/>
-    <col min="18" max="18" width="65.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="4"/>
+    <col min="2" max="2" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="4"/>
+    <col min="4" max="4" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
+    <col min="7" max="7" width="73.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="4"/>
+    <col min="12" max="12" width="89.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.88671875" style="4"/>
+    <col min="18" max="18" width="65.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="15" customFormat="1">
+    <row r="1" spans="1:29" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -7098,7 +6830,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="30.75">
+    <row r="2" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>86</v>
       </c>
@@ -7157,7 +6889,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>94</v>
       </c>
@@ -7191,7 +6923,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>96</v>
       </c>
@@ -7218,7 +6950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="G5" s="3" t="s">
         <v>98</v>
       </c>
@@ -7239,7 +6971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="G6" s="3" t="s">
         <v>99</v>
       </c>
@@ -7263,13 +6995,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z7" s="23" t="s">
-        <v>27</v>
-      </c>
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
         <v>55</v>
@@ -7278,45 +7006,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+    <row r="8" spans="1:29" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB8" s="27"/>
       <c r="AC8" s="27"/>
     </row>
-    <row r="9" spans="1:29">
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+    <row r="9" spans="1:29" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
       <c r="AC9" s="27"/>
     </row>
-    <row r="10" spans="1:29"/>
-    <row r="11" spans="1:29"/>
-    <row r="12" spans="1:29"/>
-    <row r="13" spans="1:29"/>
-    <row r="14" spans="1:29"/>
-    <row r="15" spans="1:29"/>
-    <row r="16" spans="1:29"/>
-    <row r="17"/>
-    <row r="18"/>
+    <row r="10" spans="1:29" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:29" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:29" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:29" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:29" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:29" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:29" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7329,40 +7045,40 @@
   </sheetPr>
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView topLeftCell="R5" workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="8"/>
-    <col min="4" max="4" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="8"/>
-    <col min="7" max="7" width="73.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="8"/>
-    <col min="12" max="12" width="89.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" style="8"/>
-    <col min="18" max="18" width="65.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="17.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="8"/>
+    <col min="4" max="4" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="8"/>
+    <col min="7" max="7" width="73.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="8"/>
+    <col min="12" max="12" width="89.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="8"/>
+    <col min="18" max="18" width="65.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="12" customFormat="1">
+    <row r="1" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -7434,7 +7150,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="30.75">
+    <row r="2" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>101</v>
       </c>
@@ -7491,7 +7207,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
@@ -7542,7 +7258,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>103</v>
       </c>
@@ -7589,7 +7305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>104</v>
       </c>
@@ -7632,7 +7348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="68"/>
       <c r="B6" s="67"/>
       <c r="C6" s="68"/>
@@ -7671,7 +7387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="68"/>
       <c r="B7" s="67"/>
       <c r="C7" s="68"/>
@@ -7696,9 +7412,7 @@
       <c r="V7" s="68"/>
       <c r="W7" s="68"/>
       <c r="X7" s="68"/>
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y7" s="25"/>
       <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
@@ -7708,7 +7422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="68"/>
       <c r="B8" s="67"/>
       <c r="C8" s="68"/>
@@ -7733,21 +7447,15 @@
       <c r="V8" s="68"/>
       <c r="W8" s="68"/>
       <c r="X8" s="68"/>
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB8" s="27"/>
       <c r="AC8" s="27"/>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="68"/>
       <c r="B9" s="67"/>
       <c r="C9" s="68"/>
@@ -7772,18 +7480,12 @@
       <c r="V9" s="68"/>
       <c r="W9" s="68"/>
       <c r="X9" s="68"/>
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
       <c r="AC9" s="27"/>
     </row>
   </sheetData>
@@ -7798,40 +7500,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4AAF4F-5CF1-4160-B06D-60C519E08F9C}">
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AG13" sqref="AG13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="8"/>
-    <col min="4" max="4" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="8"/>
-    <col min="7" max="7" width="73.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="8"/>
-    <col min="12" max="12" width="89.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="8"/>
-    <col min="18" max="18" width="65.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="17.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="8"/>
+    <col min="4" max="4" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="8"/>
+    <col min="7" max="7" width="73.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="8"/>
+    <col min="12" max="12" width="89.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="8"/>
+    <col min="18" max="18" width="65.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="12" customFormat="1">
+    <row r="1" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -7903,7 +7605,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="30.75">
+    <row r="2" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="46" t="s">
         <v>105</v>
       </c>
@@ -7966,7 +7668,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="60.75">
+    <row r="3" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="67"/>
       <c r="C3" s="68"/>
@@ -8017,7 +7719,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="45.75">
+    <row r="4" spans="1:29" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" s="67"/>
       <c r="C4" s="68"/>
@@ -8068,7 +7770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="76.5">
+    <row r="5" spans="1:29" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="67"/>
       <c r="C5" s="68"/>
@@ -8111,7 +7813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="30.75">
+    <row r="6" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="68"/>
       <c r="B6" s="67"/>
       <c r="C6" s="68"/>
@@ -8150,7 +7852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="68"/>
       <c r="B7" s="67"/>
       <c r="C7" s="68"/>
@@ -8175,9 +7877,7 @@
       <c r="V7" s="68"/>
       <c r="W7" s="68"/>
       <c r="X7" s="68"/>
-      <c r="Y7" s="25" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y7" s="25"/>
       <c r="Z7" s="23"/>
       <c r="AA7" s="24"/>
       <c r="AB7" s="22" t="s">
@@ -8187,7 +7887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="68"/>
       <c r="B8" s="67"/>
       <c r="C8" s="68"/>
@@ -8212,21 +7912,15 @@
       <c r="V8" s="68"/>
       <c r="W8" s="68"/>
       <c r="X8" s="68"/>
-      <c r="Y8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="27"/>
       <c r="AA8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB8" s="27"/>
       <c r="AC8" s="27"/>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="68"/>
       <c r="B9" s="67"/>
       <c r="C9" s="68"/>
@@ -8251,18 +7945,12 @@
       <c r="V9" s="68"/>
       <c r="W9" s="68"/>
       <c r="X9" s="68"/>
-      <c r="Y9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="27"/>
       <c r="AA9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AB9" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="AB9" s="27"/>
       <c r="AC9" s="27"/>
     </row>
   </sheetData>
@@ -8271,6 +7959,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000215C4F9D57D37439F8ACEF5C886EA75" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0c845befd03cfebab38c352a41d34e6a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2a5c4c29-2a22-48a5-946d-f6132279c68c" xmlns:ns3="46e2485f-814c-41c1-b1d1-92fb45bc36b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba1163b5c6633ba9dadda0673900e477" ns2:_="" ns3:_="">
     <xsd:import namespace="2a5c4c29-2a22-48a5-946d-f6132279c68c"/>
@@ -8447,29 +8150,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B85DAC82-6D37-40D8-872F-229E61782A4D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9967719E-0079-45C5-80F3-9A16D1595D17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9967719E-0079-45C5-80F3-9A16D1595D17}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F7456AA-E25E-473F-878B-9737789BB8F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F7456AA-E25E-473F-878B-9737789BB8F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B85DAC82-6D37-40D8-872F-229E61782A4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2a5c4c29-2a22-48a5-946d-f6132279c68c"/>
+    <ds:schemaRef ds:uri="46e2485f-814c-41c1-b1d1-92fb45bc36b1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>